<commit_message>
corrections and gender inclusion
</commit_message>
<xml_diff>
--- a/data/2019/contagens2019.xlsx
+++ b/data/2019/contagens2019.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735" tabRatio="758" firstSheet="5" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735" tabRatio="758" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="25.11 set + lam (centro)" sheetId="9" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="961" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="163">
   <si>
     <t>CONTAGEM VOLUMÉTRICA CLASSIFICADA — BICICLETA</t>
   </si>
@@ -1057,6 +1057,15 @@
   <si>
     <t>ci_nid</t>
   </si>
+  <si>
+    <t>lamenha 22h</t>
+  </si>
+  <si>
+    <t>lamenha pico</t>
+  </si>
+  <si>
+    <t>bento pico</t>
+  </si>
 </sst>
 </file>
 
@@ -1565,33 +1574,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1623,6 +1605,33 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1974,8 +1983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z74"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView topLeftCell="A22" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1986,76 +1995,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="21">
-      <c r="A1" s="97" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="98"/>
-      <c r="C1" s="98"/>
-      <c r="D1" s="98"/>
-      <c r="E1" s="98"/>
-      <c r="F1" s="98"/>
-      <c r="G1" s="98"/>
-      <c r="H1" s="98"/>
-      <c r="I1" s="98"/>
-      <c r="J1" s="98"/>
-      <c r="K1" s="99"/>
-      <c r="L1" s="98"/>
-      <c r="M1" s="98"/>
-      <c r="N1" s="98"/>
-      <c r="O1" s="98"/>
-      <c r="P1" s="98"/>
-      <c r="Q1" s="98"/>
-      <c r="R1" s="99"/>
+      <c r="A1" s="88" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="89"/>
+      <c r="C1" s="89"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="89"/>
+      <c r="F1" s="89"/>
+      <c r="G1" s="89"/>
+      <c r="H1" s="89"/>
+      <c r="I1" s="89"/>
+      <c r="J1" s="89"/>
+      <c r="K1" s="90"/>
+      <c r="L1" s="89"/>
+      <c r="M1" s="89"/>
+      <c r="N1" s="89"/>
+      <c r="O1" s="89"/>
+      <c r="P1" s="89"/>
+      <c r="Q1" s="89"/>
+      <c r="R1" s="90"/>
       <c r="S1" s="41"/>
       <c r="Z1" s="38"/>
     </row>
     <row r="2" spans="1:26" ht="32.1" customHeight="1">
-      <c r="A2" s="89" t="s">
+      <c r="A2" s="80" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="90"/>
-      <c r="C2" s="90"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="91" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="91"/>
-      <c r="G2" s="91"/>
-      <c r="H2" s="91"/>
-      <c r="I2" s="91"/>
-      <c r="J2" s="91"/>
-      <c r="K2" s="92"/>
+      <c r="E2" s="82" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="82"/>
+      <c r="G2" s="82"/>
+      <c r="H2" s="82"/>
+      <c r="I2" s="82"/>
+      <c r="J2" s="82"/>
+      <c r="K2" s="83"/>
       <c r="L2" s="1"/>
-      <c r="M2" s="91"/>
-      <c r="N2" s="91"/>
-      <c r="O2" s="91"/>
-      <c r="P2" s="91"/>
-      <c r="Q2" s="91"/>
-      <c r="R2" s="92"/>
+      <c r="M2" s="82"/>
+      <c r="N2" s="82"/>
+      <c r="O2" s="82"/>
+      <c r="P2" s="82"/>
+      <c r="Q2" s="82"/>
+      <c r="R2" s="83"/>
       <c r="S2" s="38"/>
       <c r="Z2" s="38"/>
     </row>
     <row r="3" spans="1:26">
-      <c r="A3" s="95" t="s">
+      <c r="A3" s="86" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="96"/>
-      <c r="C3" s="96"/>
+      <c r="B3" s="87"/>
+      <c r="C3" s="87"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="93"/>
-      <c r="J3" s="93"/>
-      <c r="K3" s="94"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="84"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="84"/>
+      <c r="J3" s="84"/>
+      <c r="K3" s="85"/>
       <c r="L3" s="2"/>
-      <c r="M3" s="93"/>
-      <c r="N3" s="93"/>
-      <c r="O3" s="93"/>
-      <c r="P3" s="93"/>
-      <c r="Q3" s="93"/>
-      <c r="R3" s="94"/>
+      <c r="M3" s="84"/>
+      <c r="N3" s="84"/>
+      <c r="O3" s="84"/>
+      <c r="P3" s="84"/>
+      <c r="Q3" s="84"/>
+      <c r="R3" s="85"/>
       <c r="S3" s="38"/>
       <c r="Z3" s="38"/>
     </row>
@@ -2082,30 +2091,30 @@
       <c r="Z4" s="38"/>
     </row>
     <row r="5" spans="1:26">
-      <c r="A5" s="80" t="s">
+      <c r="A5" s="91" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="81"/>
-      <c r="C5" s="81"/>
-      <c r="D5" s="81"/>
-      <c r="E5" s="81"/>
+      <c r="B5" s="92"/>
+      <c r="C5" s="92"/>
+      <c r="D5" s="92"/>
+      <c r="E5" s="92"/>
       <c r="F5" s="5"/>
-      <c r="G5" s="82" t="s">
+      <c r="G5" s="93" t="s">
         <v>42</v>
       </c>
-      <c r="H5" s="83"/>
-      <c r="I5" s="83"/>
-      <c r="J5" s="83"/>
-      <c r="K5" s="84"/>
+      <c r="H5" s="94"/>
+      <c r="I5" s="94"/>
+      <c r="J5" s="94"/>
+      <c r="K5" s="95"/>
       <c r="L5" s="60"/>
       <c r="M5" s="5"/>
-      <c r="N5" s="82" t="s">
+      <c r="N5" s="93" t="s">
         <v>51</v>
       </c>
-      <c r="O5" s="83"/>
-      <c r="P5" s="83"/>
-      <c r="Q5" s="83"/>
-      <c r="R5" s="84"/>
+      <c r="O5" s="94"/>
+      <c r="P5" s="94"/>
+      <c r="Q5" s="94"/>
+      <c r="R5" s="95"/>
       <c r="S5" s="38"/>
       <c r="Z5" s="38"/>
     </row>
@@ -2114,21 +2123,21 @@
       <c r="Z6" s="38"/>
     </row>
     <row r="7" spans="1:26" ht="15.95" customHeight="1">
-      <c r="B7" s="85" t="s">
+      <c r="B7" s="96" t="s">
         <v>54</v>
       </c>
-      <c r="C7" s="85"/>
-      <c r="D7" s="85"/>
-      <c r="E7" s="86" t="s">
+      <c r="C7" s="96"/>
+      <c r="D7" s="96"/>
+      <c r="E7" s="97" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="85"/>
-      <c r="G7" s="87"/>
-      <c r="H7" s="85" t="s">
+      <c r="F7" s="96"/>
+      <c r="G7" s="98"/>
+      <c r="H7" s="96" t="s">
         <v>4</v>
       </c>
-      <c r="I7" s="85"/>
-      <c r="J7" s="88"/>
+      <c r="I7" s="96"/>
+      <c r="J7" s="99"/>
       <c r="K7" s="6"/>
       <c r="L7" s="52"/>
       <c r="M7" s="71"/>
@@ -5056,18 +5065,18 @@
     <row r="74" spans="1:18" ht="16.5" thickTop="1"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="G5:K5"/>
+    <mergeCell ref="N5:R5"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="H7:J7"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="E2:K3"/>
     <mergeCell ref="M2:R3"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="L1:R1"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="G5:K5"/>
-    <mergeCell ref="N5:R5"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="H7:J7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -5078,7 +5087,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
@@ -5095,13 +5104,13 @@
       <c r="F1" s="48"/>
       <c r="G1" s="48"/>
       <c r="H1" s="49"/>
-      <c r="O1" s="98"/>
-      <c r="P1" s="98"/>
-      <c r="Q1" s="98"/>
-      <c r="R1" s="98"/>
-      <c r="S1" s="98"/>
-      <c r="T1" s="98"/>
-      <c r="U1" s="99"/>
+      <c r="O1" s="89"/>
+      <c r="P1" s="89"/>
+      <c r="Q1" s="89"/>
+      <c r="R1" s="89"/>
+      <c r="S1" s="89"/>
+      <c r="T1" s="89"/>
+      <c r="U1" s="90"/>
     </row>
     <row r="2" spans="1:21" ht="32.1" customHeight="1">
       <c r="A2" s="79" t="s">
@@ -5123,12 +5132,12 @@
       <c r="M2" s="100"/>
       <c r="N2" s="100"/>
       <c r="O2" s="1"/>
-      <c r="P2" s="91"/>
-      <c r="Q2" s="91"/>
-      <c r="R2" s="91"/>
-      <c r="S2" s="91"/>
-      <c r="T2" s="91"/>
-      <c r="U2" s="92"/>
+      <c r="P2" s="82"/>
+      <c r="Q2" s="82"/>
+      <c r="R2" s="82"/>
+      <c r="S2" s="82"/>
+      <c r="T2" s="82"/>
+      <c r="U2" s="83"/>
     </row>
     <row r="3" spans="1:21">
       <c r="A3" s="50" t="s">
@@ -5148,12 +5157,12 @@
       <c r="M3" s="100"/>
       <c r="N3" s="100"/>
       <c r="O3" s="2"/>
-      <c r="P3" s="93"/>
-      <c r="Q3" s="93"/>
-      <c r="R3" s="93"/>
-      <c r="S3" s="93"/>
-      <c r="T3" s="93"/>
-      <c r="U3" s="94"/>
+      <c r="P3" s="84"/>
+      <c r="Q3" s="84"/>
+      <c r="R3" s="84"/>
+      <c r="S3" s="84"/>
+      <c r="T3" s="84"/>
+      <c r="U3" s="85"/>
     </row>
     <row r="4" spans="1:21">
       <c r="A4" s="3"/>
@@ -5187,38 +5196,38 @@
       <c r="H5" s="46"/>
       <c r="O5" s="60"/>
       <c r="P5" s="5"/>
-      <c r="Q5" s="82" t="s">
+      <c r="Q5" s="93" t="s">
         <v>42</v>
       </c>
-      <c r="R5" s="83"/>
-      <c r="S5" s="83"/>
-      <c r="T5" s="83"/>
-      <c r="U5" s="84"/>
+      <c r="R5" s="94"/>
+      <c r="S5" s="94"/>
+      <c r="T5" s="94"/>
+      <c r="U5" s="95"/>
     </row>
     <row r="7" spans="1:21" ht="15.95" customHeight="1">
       <c r="A7" s="74" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="86" t="s">
+      <c r="B7" s="97" t="s">
         <v>108</v>
       </c>
-      <c r="C7" s="85"/>
-      <c r="D7" s="87"/>
-      <c r="E7" s="85" t="s">
+      <c r="C7" s="96"/>
+      <c r="D7" s="98"/>
+      <c r="E7" s="96" t="s">
         <v>109</v>
       </c>
-      <c r="F7" s="85"/>
-      <c r="G7" s="88"/>
-      <c r="H7" s="85" t="s">
+      <c r="F7" s="96"/>
+      <c r="G7" s="99"/>
+      <c r="H7" s="96" t="s">
         <v>110</v>
       </c>
-      <c r="I7" s="85"/>
-      <c r="J7" s="85"/>
-      <c r="K7" s="86" t="s">
+      <c r="I7" s="96"/>
+      <c r="J7" s="96"/>
+      <c r="K7" s="97" t="s">
         <v>4</v>
       </c>
-      <c r="L7" s="85"/>
-      <c r="M7" s="87"/>
+      <c r="L7" s="96"/>
+      <c r="M7" s="98"/>
       <c r="N7" s="51"/>
       <c r="O7" s="52"/>
       <c r="P7" s="52"/>
@@ -5320,7 +5329,7 @@
       <c r="L9" s="1"/>
       <c r="M9" s="13"/>
       <c r="N9" s="1">
-        <f>SUM(B9:M9)</f>
+        <f t="shared" ref="N9:N32" si="0">SUM(B9:M9)</f>
         <v>2</v>
       </c>
       <c r="O9" s="6">
@@ -5336,7 +5345,7 @@
       <c r="S9" s="18"/>
       <c r="T9" s="18"/>
       <c r="U9" s="14">
-        <f t="shared" ref="U9:U32" si="0">SUM(O9:T9)</f>
+        <f t="shared" ref="U9:U32" si="1">SUM(O9:T9)</f>
         <v>183</v>
       </c>
     </row>
@@ -5361,7 +5370,7 @@
       </c>
       <c r="M10" s="25"/>
       <c r="N10" s="1">
-        <f>SUM(B10:M10)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="O10" s="26">
@@ -5377,7 +5386,7 @@
       <c r="S10" s="22"/>
       <c r="T10" s="22"/>
       <c r="U10" s="26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>195</v>
       </c>
     </row>
@@ -5406,7 +5415,7 @@
       </c>
       <c r="M11" s="13"/>
       <c r="N11" s="1">
-        <f>SUM(B11:M11)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="O11" s="14">
@@ -5424,7 +5433,7 @@
       </c>
       <c r="T11" s="15"/>
       <c r="U11" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>227</v>
       </c>
     </row>
@@ -5449,7 +5458,7 @@
       <c r="L12" s="23"/>
       <c r="M12" s="25"/>
       <c r="N12" s="1">
-        <f>SUM(B12:M12)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="O12" s="26">
@@ -5467,7 +5476,7 @@
       </c>
       <c r="T12" s="22"/>
       <c r="U12" s="26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>168</v>
       </c>
     </row>
@@ -5490,7 +5499,7 @@
       <c r="L13" s="1"/>
       <c r="M13" s="13"/>
       <c r="N13" s="1">
-        <f>SUM(B13:M13)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="O13" s="14">
@@ -5508,7 +5517,7 @@
       <c r="S13" s="15"/>
       <c r="T13" s="15"/>
       <c r="U13" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>167</v>
       </c>
     </row>
@@ -5529,7 +5538,7 @@
       <c r="L14" s="23"/>
       <c r="M14" s="25"/>
       <c r="N14" s="1">
-        <f>SUM(B14:M14)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O14" s="26">
@@ -5547,7 +5556,7 @@
       </c>
       <c r="T14" s="22"/>
       <c r="U14" s="26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>142</v>
       </c>
     </row>
@@ -5576,7 +5585,7 @@
       <c r="L15" s="1"/>
       <c r="M15" s="13"/>
       <c r="N15" s="1">
-        <f>SUM(B15:M15)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="O15" s="14">
@@ -5592,7 +5601,7 @@
       <c r="S15" s="15"/>
       <c r="T15" s="15"/>
       <c r="U15" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>161</v>
       </c>
     </row>
@@ -5615,7 +5624,7 @@
       <c r="L16" s="23"/>
       <c r="M16" s="25"/>
       <c r="N16" s="1">
-        <f>SUM(B16:M16)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="O16" s="26">
@@ -5631,7 +5640,7 @@
       <c r="S16" s="22"/>
       <c r="T16" s="22"/>
       <c r="U16" s="26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>163</v>
       </c>
     </row>
@@ -5652,7 +5661,7 @@
       <c r="L17" s="1"/>
       <c r="M17" s="13"/>
       <c r="N17" s="1">
-        <f>SUM(B17:M17)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O17" s="14">
@@ -5672,7 +5681,7 @@
       </c>
       <c r="T17" s="15"/>
       <c r="U17" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>158</v>
       </c>
     </row>
@@ -5701,7 +5710,7 @@
       <c r="L18" s="23"/>
       <c r="M18" s="25"/>
       <c r="N18" s="1">
-        <f>SUM(B18:M18)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="O18" s="26">
@@ -5717,7 +5726,7 @@
       <c r="S18" s="22"/>
       <c r="T18" s="22"/>
       <c r="U18" s="26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>133</v>
       </c>
     </row>
@@ -5742,7 +5751,7 @@
       <c r="L19" s="1"/>
       <c r="M19" s="13"/>
       <c r="N19" s="1">
-        <f>SUM(B19:M19)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="O19" s="14">
@@ -5760,7 +5769,7 @@
       <c r="S19" s="15"/>
       <c r="T19" s="15"/>
       <c r="U19" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>198</v>
       </c>
     </row>
@@ -5783,7 +5792,7 @@
       <c r="L20" s="30"/>
       <c r="M20" s="32"/>
       <c r="N20" s="1">
-        <f>SUM(B20:M20)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="O20" s="33">
@@ -5803,7 +5812,7 @@
       </c>
       <c r="T20" s="29"/>
       <c r="U20" s="33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>212</v>
       </c>
     </row>
@@ -5832,7 +5841,7 @@
       <c r="L21" s="1"/>
       <c r="M21" s="13"/>
       <c r="N21" s="1">
-        <f>SUM(B21:M21)</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="O21" s="6">
@@ -5850,7 +5859,7 @@
       <c r="S21" s="18"/>
       <c r="T21" s="18"/>
       <c r="U21" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>259</v>
       </c>
     </row>
@@ -5879,7 +5888,7 @@
       </c>
       <c r="M22" s="25"/>
       <c r="N22" s="1">
-        <f>SUM(B22:M22)</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="O22" s="26">
@@ -5897,7 +5906,7 @@
       <c r="S22" s="22"/>
       <c r="T22" s="22"/>
       <c r="U22" s="26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>259</v>
       </c>
     </row>
@@ -5924,7 +5933,7 @@
       <c r="L23" s="1"/>
       <c r="M23" s="13"/>
       <c r="N23" s="1">
-        <f>SUM(B23:M23)</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="O23" s="14">
@@ -5942,7 +5951,7 @@
       <c r="S23" s="15"/>
       <c r="T23" s="15"/>
       <c r="U23" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>288</v>
       </c>
     </row>
@@ -5973,7 +5982,7 @@
       </c>
       <c r="M24" s="25"/>
       <c r="N24" s="1">
-        <f>SUM(B24:M24)</f>
+        <f t="shared" si="0"/>
         <v>36</v>
       </c>
       <c r="O24" s="26">
@@ -5993,7 +6002,7 @@
       </c>
       <c r="T24" s="22"/>
       <c r="U24" s="26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>331</v>
       </c>
     </row>
@@ -6024,7 +6033,7 @@
       </c>
       <c r="M25" s="13"/>
       <c r="N25" s="1">
-        <f>SUM(B25:M25)</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="O25" s="14">
@@ -6042,7 +6051,7 @@
       <c r="S25" s="15"/>
       <c r="T25" s="15"/>
       <c r="U25" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>343</v>
       </c>
     </row>
@@ -6071,7 +6080,7 @@
       <c r="L26" s="23"/>
       <c r="M26" s="25"/>
       <c r="N26" s="1">
-        <f>SUM(B26:M26)</f>
+        <f t="shared" si="0"/>
         <v>37</v>
       </c>
       <c r="O26" s="26">
@@ -6089,7 +6098,7 @@
       <c r="S26" s="22"/>
       <c r="T26" s="22"/>
       <c r="U26" s="26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>349</v>
       </c>
     </row>
@@ -6116,7 +6125,7 @@
       <c r="L27" s="1"/>
       <c r="M27" s="13"/>
       <c r="N27" s="1">
-        <f>SUM(B27:M27)</f>
+        <f t="shared" si="0"/>
         <v>34</v>
       </c>
       <c r="O27" s="14">
@@ -6134,7 +6143,7 @@
       <c r="S27" s="15"/>
       <c r="T27" s="15"/>
       <c r="U27" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>359</v>
       </c>
     </row>
@@ -6163,7 +6172,7 @@
       </c>
       <c r="M28" s="25"/>
       <c r="N28" s="1">
-        <f>SUM(B28:M28)</f>
+        <f t="shared" si="0"/>
         <v>47</v>
       </c>
       <c r="O28" s="26">
@@ -6181,7 +6190,7 @@
       <c r="S28" s="22"/>
       <c r="T28" s="22"/>
       <c r="U28" s="26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>325</v>
       </c>
     </row>
@@ -6206,7 +6215,7 @@
       <c r="L29" s="1"/>
       <c r="M29" s="13"/>
       <c r="N29" s="1">
-        <f>SUM(B29:M29)</f>
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="O29" s="14">
@@ -6224,7 +6233,7 @@
       <c r="S29" s="15"/>
       <c r="T29" s="15"/>
       <c r="U29" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>338</v>
       </c>
     </row>
@@ -6255,7 +6264,7 @@
       </c>
       <c r="M30" s="25"/>
       <c r="N30" s="1">
-        <f>SUM(B30:M30)</f>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="O30" s="26">
@@ -6271,7 +6280,7 @@
       <c r="S30" s="22"/>
       <c r="T30" s="22"/>
       <c r="U30" s="26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>262</v>
       </c>
     </row>
@@ -6300,7 +6309,7 @@
       <c r="L31" s="1"/>
       <c r="M31" s="13"/>
       <c r="N31" s="1">
-        <f>SUM(B31:M31)</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="O31" s="14">
@@ -6318,7 +6327,7 @@
       <c r="S31" s="15"/>
       <c r="T31" s="15"/>
       <c r="U31" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>264</v>
       </c>
     </row>
@@ -6347,7 +6356,7 @@
       </c>
       <c r="M32" s="32"/>
       <c r="N32" s="1">
-        <f>SUM(B32:M32)</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="O32" s="33">
@@ -6365,7 +6374,7 @@
       <c r="S32" s="29"/>
       <c r="T32" s="29"/>
       <c r="U32" s="33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>251</v>
       </c>
     </row>
@@ -6418,11 +6427,11 @@
       <c r="R1" s="106"/>
     </row>
     <row r="2" spans="1:18" ht="32.1" customHeight="1">
-      <c r="A2" s="89" t="s">
+      <c r="A2" s="80" t="s">
         <v>116</v>
       </c>
-      <c r="B2" s="90"/>
-      <c r="C2" s="90"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
       <c r="D2" s="1"/>
       <c r="E2" s="100" t="s">
         <v>117</v>
@@ -6442,11 +6451,11 @@
       <c r="R2" s="101"/>
     </row>
     <row r="3" spans="1:18">
-      <c r="A3" s="95" t="s">
+      <c r="A3" s="86" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="96"/>
-      <c r="C3" s="96"/>
+      <c r="B3" s="87"/>
+      <c r="C3" s="87"/>
       <c r="D3" s="2"/>
       <c r="E3" s="102"/>
       <c r="F3" s="102"/>
@@ -6484,30 +6493,30 @@
       <c r="R4" s="4"/>
     </row>
     <row r="5" spans="1:18">
-      <c r="A5" s="80" t="s">
+      <c r="A5" s="91" t="s">
         <v>122</v>
       </c>
-      <c r="B5" s="81"/>
-      <c r="C5" s="81"/>
-      <c r="D5" s="81"/>
-      <c r="E5" s="81"/>
+      <c r="B5" s="92"/>
+      <c r="C5" s="92"/>
+      <c r="D5" s="92"/>
+      <c r="E5" s="92"/>
       <c r="F5" s="5"/>
-      <c r="G5" s="81" t="s">
+      <c r="G5" s="92" t="s">
         <v>123</v>
       </c>
-      <c r="H5" s="83"/>
-      <c r="I5" s="83"/>
-      <c r="J5" s="83"/>
-      <c r="K5" s="84"/>
+      <c r="H5" s="94"/>
+      <c r="I5" s="94"/>
+      <c r="J5" s="94"/>
+      <c r="K5" s="95"/>
       <c r="L5" s="60"/>
       <c r="M5" s="5"/>
-      <c r="N5" s="81" t="s">
+      <c r="N5" s="92" t="s">
         <v>124</v>
       </c>
-      <c r="O5" s="83"/>
-      <c r="P5" s="83"/>
-      <c r="Q5" s="83"/>
-      <c r="R5" s="84"/>
+      <c r="O5" s="94"/>
+      <c r="P5" s="94"/>
+      <c r="Q5" s="94"/>
+      <c r="R5" s="95"/>
     </row>
     <row r="8" spans="1:18" ht="31.5">
       <c r="A8" s="74" t="s">
@@ -7792,11 +7801,11 @@
       <c r="R1" s="106"/>
     </row>
     <row r="2" spans="1:18" ht="32.1" customHeight="1">
-      <c r="A2" s="89" t="s">
+      <c r="A2" s="80" t="s">
         <v>116</v>
       </c>
-      <c r="B2" s="90"/>
-      <c r="C2" s="90"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
       <c r="D2" s="1"/>
       <c r="E2" s="100" t="s">
         <v>117</v>
@@ -7816,11 +7825,11 @@
       <c r="R2" s="101"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" customHeight="1">
-      <c r="A3" s="95" t="s">
+      <c r="A3" s="86" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="96"/>
-      <c r="C3" s="96"/>
+      <c r="B3" s="87"/>
+      <c r="C3" s="87"/>
       <c r="D3" s="2"/>
       <c r="E3" s="102"/>
       <c r="F3" s="102"/>
@@ -7858,30 +7867,30 @@
       <c r="R4" s="4"/>
     </row>
     <row r="5" spans="1:18">
-      <c r="A5" s="80" t="s">
+      <c r="A5" s="91" t="s">
         <v>118</v>
       </c>
-      <c r="B5" s="81"/>
-      <c r="C5" s="81"/>
-      <c r="D5" s="81"/>
-      <c r="E5" s="81"/>
+      <c r="B5" s="92"/>
+      <c r="C5" s="92"/>
+      <c r="D5" s="92"/>
+      <c r="E5" s="92"/>
       <c r="F5" s="5"/>
-      <c r="G5" s="81" t="s">
+      <c r="G5" s="92" t="s">
         <v>119</v>
       </c>
-      <c r="H5" s="83"/>
-      <c r="I5" s="83"/>
-      <c r="J5" s="83"/>
-      <c r="K5" s="84"/>
+      <c r="H5" s="94"/>
+      <c r="I5" s="94"/>
+      <c r="J5" s="94"/>
+      <c r="K5" s="95"/>
       <c r="L5" s="60"/>
       <c r="M5" s="5"/>
-      <c r="N5" s="81" t="s">
+      <c r="N5" s="92" t="s">
         <v>120</v>
       </c>
-      <c r="O5" s="83"/>
-      <c r="P5" s="83"/>
-      <c r="Q5" s="83"/>
-      <c r="R5" s="84"/>
+      <c r="O5" s="94"/>
+      <c r="P5" s="94"/>
+      <c r="Q5" s="94"/>
+      <c r="R5" s="95"/>
     </row>
     <row r="7" spans="1:18" ht="15.95" customHeight="1">
       <c r="A7" s="61" t="s">
@@ -9177,8 +9186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:D8"/>
+    <sheetView topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I21" activeCellId="2" sqref="C21:C32 F21:F32 I21:I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -9399,11 +9408,11 @@
       <c r="R1" s="106"/>
     </row>
     <row r="2" spans="1:18" ht="32.1" customHeight="1">
-      <c r="A2" s="89" t="s">
+      <c r="A2" s="80" t="s">
         <v>125</v>
       </c>
-      <c r="B2" s="90"/>
-      <c r="C2" s="90"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
       <c r="D2" s="1"/>
       <c r="E2" s="107" t="s">
         <v>126</v>
@@ -9423,11 +9432,11 @@
       <c r="R2" s="108"/>
     </row>
     <row r="3" spans="1:18" ht="27.75" customHeight="1">
-      <c r="A3" s="95" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="96"/>
-      <c r="C3" s="96"/>
+      <c r="A3" s="86" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="87"/>
+      <c r="C3" s="87"/>
       <c r="D3" s="2"/>
       <c r="E3" s="109"/>
       <c r="F3" s="109"/>
@@ -9465,30 +9474,30 @@
       <c r="R4" s="4"/>
     </row>
     <row r="5" spans="1:18">
-      <c r="A5" s="80" t="s">
+      <c r="A5" s="91" t="s">
         <v>122</v>
       </c>
-      <c r="B5" s="81"/>
-      <c r="C5" s="81"/>
-      <c r="D5" s="81"/>
-      <c r="E5" s="81"/>
+      <c r="B5" s="92"/>
+      <c r="C5" s="92"/>
+      <c r="D5" s="92"/>
+      <c r="E5" s="92"/>
       <c r="F5" s="5"/>
-      <c r="G5" s="81" t="s">
+      <c r="G5" s="92" t="s">
         <v>129</v>
       </c>
-      <c r="H5" s="83"/>
-      <c r="I5" s="83"/>
-      <c r="J5" s="83"/>
-      <c r="K5" s="84"/>
+      <c r="H5" s="94"/>
+      <c r="I5" s="94"/>
+      <c r="J5" s="94"/>
+      <c r="K5" s="95"/>
       <c r="L5" s="60"/>
       <c r="M5" s="5"/>
-      <c r="N5" s="82" t="s">
+      <c r="N5" s="93" t="s">
         <v>53</v>
       </c>
-      <c r="O5" s="83"/>
-      <c r="P5" s="83"/>
-      <c r="Q5" s="83"/>
-      <c r="R5" s="84"/>
+      <c r="O5" s="94"/>
+      <c r="P5" s="94"/>
+      <c r="Q5" s="94"/>
+      <c r="R5" s="95"/>
     </row>
     <row r="6" spans="1:18">
       <c r="B6" s="2" t="s">
@@ -11006,8 +11015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:D8"/>
+    <sheetView topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C21" activeCellId="2" sqref="I21:I32 F21:F33 C21:C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -11228,11 +11237,11 @@
       <c r="R1" s="106"/>
     </row>
     <row r="2" spans="1:18" ht="32.1" customHeight="1">
-      <c r="A2" s="89" t="s">
+      <c r="A2" s="80" t="s">
         <v>125</v>
       </c>
-      <c r="B2" s="90"/>
-      <c r="C2" s="90"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
       <c r="D2" s="1"/>
       <c r="E2" s="107" t="s">
         <v>126</v>
@@ -11252,11 +11261,11 @@
       <c r="R2" s="108"/>
     </row>
     <row r="3" spans="1:18" ht="23.25" customHeight="1">
-      <c r="A3" s="95" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="96"/>
-      <c r="C3" s="96"/>
+      <c r="A3" s="86" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="87"/>
+      <c r="C3" s="87"/>
       <c r="D3" s="2"/>
       <c r="E3" s="109"/>
       <c r="F3" s="109"/>
@@ -11294,30 +11303,30 @@
       <c r="R4" s="4"/>
     </row>
     <row r="5" spans="1:18">
-      <c r="A5" s="80" t="s">
+      <c r="A5" s="91" t="s">
         <v>118</v>
       </c>
-      <c r="B5" s="81"/>
-      <c r="C5" s="81"/>
-      <c r="D5" s="81"/>
-      <c r="E5" s="81"/>
+      <c r="B5" s="92"/>
+      <c r="C5" s="92"/>
+      <c r="D5" s="92"/>
+      <c r="E5" s="92"/>
       <c r="F5" s="5"/>
-      <c r="G5" s="81" t="s">
+      <c r="G5" s="92" t="s">
         <v>127</v>
       </c>
-      <c r="H5" s="83"/>
-      <c r="I5" s="83"/>
-      <c r="J5" s="83"/>
-      <c r="K5" s="84"/>
+      <c r="H5" s="94"/>
+      <c r="I5" s="94"/>
+      <c r="J5" s="94"/>
+      <c r="K5" s="95"/>
       <c r="L5" s="60"/>
       <c r="M5" s="5"/>
-      <c r="N5" s="81" t="s">
+      <c r="N5" s="92" t="s">
         <v>128</v>
       </c>
-      <c r="O5" s="83"/>
-      <c r="P5" s="83"/>
-      <c r="Q5" s="83"/>
-      <c r="R5" s="84"/>
+      <c r="O5" s="94"/>
+      <c r="P5" s="94"/>
+      <c r="Q5" s="94"/>
+      <c r="R5" s="95"/>
     </row>
     <row r="6" spans="1:18">
       <c r="B6" s="2" t="s">
@@ -12836,7 +12845,7 @@
   <dimension ref="A1:R32"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+      <selection activeCell="K21" sqref="K21:K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -12864,50 +12873,50 @@
       <c r="R1" s="106"/>
     </row>
     <row r="2" spans="1:18" ht="32.1" customHeight="1">
-      <c r="A2" s="89" t="s">
+      <c r="A2" s="80" t="s">
         <v>130</v>
       </c>
-      <c r="B2" s="90"/>
-      <c r="C2" s="90"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="91" t="s">
+      <c r="E2" s="82" t="s">
         <v>43</v>
       </c>
-      <c r="F2" s="91"/>
-      <c r="G2" s="91"/>
-      <c r="H2" s="91"/>
-      <c r="I2" s="91"/>
-      <c r="J2" s="91"/>
-      <c r="K2" s="92"/>
+      <c r="F2" s="82"/>
+      <c r="G2" s="82"/>
+      <c r="H2" s="82"/>
+      <c r="I2" s="82"/>
+      <c r="J2" s="82"/>
+      <c r="K2" s="83"/>
       <c r="L2" s="1"/>
-      <c r="M2" s="91"/>
-      <c r="N2" s="91"/>
-      <c r="O2" s="91"/>
-      <c r="P2" s="91"/>
-      <c r="Q2" s="91"/>
-      <c r="R2" s="92"/>
+      <c r="M2" s="82"/>
+      <c r="N2" s="82"/>
+      <c r="O2" s="82"/>
+      <c r="P2" s="82"/>
+      <c r="Q2" s="82"/>
+      <c r="R2" s="83"/>
     </row>
     <row r="3" spans="1:18">
-      <c r="A3" s="95" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="96"/>
-      <c r="C3" s="96"/>
+      <c r="A3" s="86" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="87"/>
+      <c r="C3" s="87"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="93"/>
-      <c r="J3" s="93"/>
-      <c r="K3" s="94"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="84"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="84"/>
+      <c r="J3" s="84"/>
+      <c r="K3" s="85"/>
       <c r="L3" s="2"/>
-      <c r="M3" s="93"/>
-      <c r="N3" s="93"/>
-      <c r="O3" s="93"/>
-      <c r="P3" s="93"/>
-      <c r="Q3" s="93"/>
-      <c r="R3" s="94"/>
+      <c r="M3" s="84"/>
+      <c r="N3" s="84"/>
+      <c r="O3" s="84"/>
+      <c r="P3" s="84"/>
+      <c r="Q3" s="84"/>
+      <c r="R3" s="85"/>
     </row>
     <row r="4" spans="1:18">
       <c r="A4" s="3"/>
@@ -12930,30 +12939,30 @@
       <c r="R4" s="4"/>
     </row>
     <row r="5" spans="1:18">
-      <c r="A5" s="80" t="s">
+      <c r="A5" s="91" t="s">
         <v>122</v>
       </c>
-      <c r="B5" s="81"/>
-      <c r="C5" s="81"/>
-      <c r="D5" s="81"/>
-      <c r="E5" s="81"/>
+      <c r="B5" s="92"/>
+      <c r="C5" s="92"/>
+      <c r="D5" s="92"/>
+      <c r="E5" s="92"/>
       <c r="F5" s="5"/>
-      <c r="G5" s="82" t="s">
+      <c r="G5" s="93" t="s">
         <v>42</v>
       </c>
-      <c r="H5" s="83"/>
-      <c r="I5" s="83"/>
-      <c r="J5" s="83"/>
-      <c r="K5" s="84"/>
+      <c r="H5" s="94"/>
+      <c r="I5" s="94"/>
+      <c r="J5" s="94"/>
+      <c r="K5" s="95"/>
       <c r="L5" s="60"/>
       <c r="M5" s="5"/>
-      <c r="N5" s="82" t="s">
+      <c r="N5" s="93" t="s">
         <v>40</v>
       </c>
-      <c r="O5" s="83"/>
-      <c r="P5" s="83"/>
-      <c r="Q5" s="83"/>
-      <c r="R5" s="84"/>
+      <c r="O5" s="94"/>
+      <c r="P5" s="94"/>
+      <c r="Q5" s="94"/>
+      <c r="R5" s="95"/>
     </row>
     <row r="7" spans="1:18" ht="15.95" customHeight="1">
       <c r="A7" s="74" t="s">
@@ -14027,7 +14036,7 @@
   <dimension ref="A1:R32"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="K21" sqref="K21:K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -14055,50 +14064,50 @@
       <c r="R1" s="106"/>
     </row>
     <row r="2" spans="1:18" ht="32.1" customHeight="1">
-      <c r="A2" s="89" t="s">
+      <c r="A2" s="80" t="s">
         <v>130</v>
       </c>
-      <c r="B2" s="90"/>
-      <c r="C2" s="90"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="91" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="91"/>
-      <c r="G2" s="91"/>
-      <c r="H2" s="91"/>
-      <c r="I2" s="91"/>
-      <c r="J2" s="91"/>
-      <c r="K2" s="92"/>
+      <c r="E2" s="82" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="82"/>
+      <c r="G2" s="82"/>
+      <c r="H2" s="82"/>
+      <c r="I2" s="82"/>
+      <c r="J2" s="82"/>
+      <c r="K2" s="83"/>
       <c r="L2" s="1"/>
-      <c r="M2" s="91"/>
-      <c r="N2" s="91"/>
-      <c r="O2" s="91"/>
-      <c r="P2" s="91"/>
-      <c r="Q2" s="91"/>
-      <c r="R2" s="92"/>
+      <c r="M2" s="82"/>
+      <c r="N2" s="82"/>
+      <c r="O2" s="82"/>
+      <c r="P2" s="82"/>
+      <c r="Q2" s="82"/>
+      <c r="R2" s="83"/>
     </row>
     <row r="3" spans="1:18">
-      <c r="A3" s="95" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="96"/>
-      <c r="C3" s="96"/>
+      <c r="A3" s="86" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="87"/>
+      <c r="C3" s="87"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="93"/>
-      <c r="J3" s="93"/>
-      <c r="K3" s="94"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="84"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="84"/>
+      <c r="J3" s="84"/>
+      <c r="K3" s="85"/>
       <c r="L3" s="2"/>
-      <c r="M3" s="93"/>
-      <c r="N3" s="93"/>
-      <c r="O3" s="93"/>
-      <c r="P3" s="93"/>
-      <c r="Q3" s="93"/>
-      <c r="R3" s="94"/>
+      <c r="M3" s="84"/>
+      <c r="N3" s="84"/>
+      <c r="O3" s="84"/>
+      <c r="P3" s="84"/>
+      <c r="Q3" s="84"/>
+      <c r="R3" s="85"/>
     </row>
     <row r="4" spans="1:18">
       <c r="A4" s="3"/>
@@ -14121,30 +14130,30 @@
       <c r="R4" s="4"/>
     </row>
     <row r="5" spans="1:18">
-      <c r="A5" s="80" t="s">
+      <c r="A5" s="91" t="s">
         <v>118</v>
       </c>
-      <c r="B5" s="81"/>
-      <c r="C5" s="81"/>
-      <c r="D5" s="81"/>
-      <c r="E5" s="81"/>
+      <c r="B5" s="92"/>
+      <c r="C5" s="92"/>
+      <c r="D5" s="92"/>
+      <c r="E5" s="92"/>
       <c r="F5" s="5"/>
-      <c r="G5" s="82" t="s">
+      <c r="G5" s="93" t="s">
         <v>44</v>
       </c>
-      <c r="H5" s="83"/>
-      <c r="I5" s="83"/>
-      <c r="J5" s="83"/>
-      <c r="K5" s="84"/>
+      <c r="H5" s="94"/>
+      <c r="I5" s="94"/>
+      <c r="J5" s="94"/>
+      <c r="K5" s="95"/>
       <c r="L5" s="60"/>
       <c r="M5" s="5"/>
-      <c r="N5" s="82" t="s">
+      <c r="N5" s="93" t="s">
         <v>41</v>
       </c>
-      <c r="O5" s="83"/>
-      <c r="P5" s="83"/>
-      <c r="Q5" s="83"/>
-      <c r="R5" s="84"/>
+      <c r="O5" s="94"/>
+      <c r="P5" s="94"/>
+      <c r="Q5" s="94"/>
+      <c r="R5" s="95"/>
     </row>
     <row r="7" spans="1:18" ht="15.95" customHeight="1">
       <c r="A7" s="74" t="s">
@@ -15237,8 +15246,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z72"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView topLeftCell="A25" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="V52" sqref="V52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -15249,43 +15258,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="20.25">
-      <c r="A1" s="97" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="98"/>
-      <c r="C1" s="98"/>
-      <c r="D1" s="98"/>
-      <c r="E1" s="98"/>
-      <c r="F1" s="98"/>
-      <c r="G1" s="98"/>
-      <c r="H1" s="98"/>
-      <c r="I1" s="98"/>
-      <c r="J1" s="98"/>
-      <c r="K1" s="99"/>
-      <c r="L1" s="98"/>
-      <c r="M1" s="98"/>
-      <c r="N1" s="98"/>
-      <c r="O1" s="98"/>
-      <c r="P1" s="98"/>
-      <c r="Q1" s="98"/>
-      <c r="R1" s="99"/>
+      <c r="A1" s="88" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="89"/>
+      <c r="C1" s="89"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="89"/>
+      <c r="F1" s="89"/>
+      <c r="G1" s="89"/>
+      <c r="H1" s="89"/>
+      <c r="I1" s="89"/>
+      <c r="J1" s="89"/>
+      <c r="K1" s="90"/>
+      <c r="L1" s="89"/>
+      <c r="M1" s="89"/>
+      <c r="N1" s="89"/>
+      <c r="O1" s="89"/>
+      <c r="P1" s="89"/>
+      <c r="Q1" s="89"/>
+      <c r="R1" s="90"/>
     </row>
     <row r="2" spans="1:26" ht="32.1" customHeight="1">
-      <c r="A2" s="89" t="s">
+      <c r="A2" s="80" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="90"/>
-      <c r="C2" s="90"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="91" t="s">
+      <c r="E2" s="82" t="s">
         <v>104</v>
       </c>
-      <c r="F2" s="91"/>
-      <c r="G2" s="91"/>
-      <c r="H2" s="91"/>
-      <c r="I2" s="91"/>
-      <c r="J2" s="91"/>
-      <c r="K2" s="92"/>
+      <c r="F2" s="82"/>
+      <c r="G2" s="82"/>
+      <c r="H2" s="82"/>
+      <c r="I2" s="82"/>
+      <c r="J2" s="82"/>
+      <c r="K2" s="83"/>
       <c r="L2" s="1"/>
       <c r="M2" s="100"/>
       <c r="N2" s="100"/>
@@ -15295,19 +15304,19 @@
       <c r="R2" s="101"/>
     </row>
     <row r="3" spans="1:26">
-      <c r="A3" s="95" t="s">
+      <c r="A3" s="86" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="96"/>
-      <c r="C3" s="96"/>
+      <c r="B3" s="87"/>
+      <c r="C3" s="87"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="93"/>
-      <c r="J3" s="93"/>
-      <c r="K3" s="94"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="84"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="84"/>
+      <c r="J3" s="84"/>
+      <c r="K3" s="85"/>
       <c r="L3" s="2"/>
       <c r="M3" s="102"/>
       <c r="N3" s="102"/>
@@ -15337,30 +15346,30 @@
       <c r="R4" s="4"/>
     </row>
     <row r="5" spans="1:26">
-      <c r="A5" s="80" t="s">
+      <c r="A5" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="81"/>
-      <c r="C5" s="81"/>
-      <c r="D5" s="81"/>
-      <c r="E5" s="81"/>
+      <c r="B5" s="92"/>
+      <c r="C5" s="92"/>
+      <c r="D5" s="92"/>
+      <c r="E5" s="92"/>
       <c r="F5" s="5"/>
-      <c r="G5" s="82" t="s">
+      <c r="G5" s="93" t="s">
         <v>42</v>
       </c>
-      <c r="H5" s="83"/>
-      <c r="I5" s="83"/>
-      <c r="J5" s="83"/>
-      <c r="K5" s="84"/>
+      <c r="H5" s="94"/>
+      <c r="I5" s="94"/>
+      <c r="J5" s="94"/>
+      <c r="K5" s="95"/>
       <c r="L5" s="60"/>
       <c r="M5" s="5"/>
-      <c r="N5" s="82" t="s">
+      <c r="N5" s="93" t="s">
         <v>62</v>
       </c>
-      <c r="O5" s="83"/>
-      <c r="P5" s="83"/>
-      <c r="Q5" s="83"/>
-      <c r="R5" s="84"/>
+      <c r="O5" s="94"/>
+      <c r="P5" s="94"/>
+      <c r="Q5" s="94"/>
+      <c r="R5" s="95"/>
     </row>
     <row r="7" spans="1:26" ht="15.95" customHeight="1">
       <c r="B7" s="51" t="s">
@@ -17405,8 +17414,13 @@
       </c>
       <c r="S49" s="38"/>
       <c r="T49" s="38"/>
-      <c r="U49" s="38"/>
-      <c r="V49" s="38"/>
+      <c r="U49" s="38" t="s">
+        <v>160</v>
+      </c>
+      <c r="V49" s="38">
+        <f>262+198+13+38+52</f>
+        <v>563</v>
+      </c>
       <c r="W49" s="38"/>
       <c r="X49" s="38"/>
       <c r="Y49" s="38"/>
@@ -17453,8 +17467,13 @@
       </c>
       <c r="S50" s="38"/>
       <c r="T50" s="38"/>
-      <c r="U50" s="38"/>
-      <c r="V50" s="38"/>
+      <c r="U50" s="38" t="s">
+        <v>161</v>
+      </c>
+      <c r="V50" s="38">
+        <f>289+8+29+184+4+46</f>
+        <v>560</v>
+      </c>
       <c r="W50" s="38"/>
       <c r="X50" s="38"/>
       <c r="Y50" s="38"/>
@@ -17505,8 +17524,13 @@
       </c>
       <c r="S51" s="38"/>
       <c r="T51" s="38"/>
-      <c r="U51" s="38"/>
-      <c r="V51" s="38"/>
+      <c r="U51" s="38" t="s">
+        <v>162</v>
+      </c>
+      <c r="V51" s="38">
+        <f>81+41+114+7+21</f>
+        <v>264</v>
+      </c>
       <c r="W51" s="38"/>
       <c r="X51" s="38"/>
       <c r="Y51" s="38"/>
@@ -18463,79 +18487,79 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I21" activeCellId="1" sqref="C21:C32 I21:I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:18" ht="20.25">
-      <c r="A1" s="97" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="98"/>
-      <c r="C1" s="98"/>
-      <c r="D1" s="98"/>
-      <c r="E1" s="98"/>
-      <c r="F1" s="98"/>
-      <c r="G1" s="98"/>
-      <c r="H1" s="98"/>
-      <c r="I1" s="98"/>
-      <c r="J1" s="98"/>
-      <c r="K1" s="99"/>
-      <c r="L1" s="98"/>
-      <c r="M1" s="98"/>
-      <c r="N1" s="98"/>
-      <c r="O1" s="98"/>
-      <c r="P1" s="98"/>
-      <c r="Q1" s="98"/>
-      <c r="R1" s="99"/>
+      <c r="A1" s="88" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="89"/>
+      <c r="C1" s="89"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="89"/>
+      <c r="F1" s="89"/>
+      <c r="G1" s="89"/>
+      <c r="H1" s="89"/>
+      <c r="I1" s="89"/>
+      <c r="J1" s="89"/>
+      <c r="K1" s="90"/>
+      <c r="L1" s="89"/>
+      <c r="M1" s="89"/>
+      <c r="N1" s="89"/>
+      <c r="O1" s="89"/>
+      <c r="P1" s="89"/>
+      <c r="Q1" s="89"/>
+      <c r="R1" s="90"/>
     </row>
     <row r="2" spans="1:18" ht="32.1" customHeight="1">
-      <c r="A2" s="89" t="s">
+      <c r="A2" s="80" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="90"/>
-      <c r="C2" s="90"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="91" t="s">
+      <c r="E2" s="82" t="s">
         <v>47</v>
       </c>
-      <c r="F2" s="91"/>
-      <c r="G2" s="91"/>
-      <c r="H2" s="91"/>
-      <c r="I2" s="91"/>
-      <c r="J2" s="91"/>
-      <c r="K2" s="92"/>
+      <c r="F2" s="82"/>
+      <c r="G2" s="82"/>
+      <c r="H2" s="82"/>
+      <c r="I2" s="82"/>
+      <c r="J2" s="82"/>
+      <c r="K2" s="83"/>
       <c r="L2" s="1"/>
-      <c r="M2" s="91"/>
-      <c r="N2" s="91"/>
-      <c r="O2" s="91"/>
-      <c r="P2" s="91"/>
-      <c r="Q2" s="91"/>
-      <c r="R2" s="92"/>
+      <c r="M2" s="82"/>
+      <c r="N2" s="82"/>
+      <c r="O2" s="82"/>
+      <c r="P2" s="82"/>
+      <c r="Q2" s="82"/>
+      <c r="R2" s="83"/>
     </row>
     <row r="3" spans="1:18">
-      <c r="A3" s="95" t="s">
+      <c r="A3" s="86" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="96"/>
-      <c r="C3" s="96"/>
+      <c r="B3" s="87"/>
+      <c r="C3" s="87"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="93"/>
-      <c r="J3" s="93"/>
-      <c r="K3" s="94"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="84"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="84"/>
+      <c r="J3" s="84"/>
+      <c r="K3" s="85"/>
       <c r="L3" s="2"/>
-      <c r="M3" s="93"/>
-      <c r="N3" s="93"/>
-      <c r="O3" s="93"/>
-      <c r="P3" s="93"/>
-      <c r="Q3" s="93"/>
-      <c r="R3" s="94"/>
+      <c r="M3" s="84"/>
+      <c r="N3" s="84"/>
+      <c r="O3" s="84"/>
+      <c r="P3" s="84"/>
+      <c r="Q3" s="84"/>
+      <c r="R3" s="85"/>
     </row>
     <row r="4" spans="1:18">
       <c r="A4" s="3"/>
@@ -18558,30 +18582,30 @@
       <c r="R4" s="4"/>
     </row>
     <row r="5" spans="1:18">
-      <c r="A5" s="80" t="s">
+      <c r="A5" s="91" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="81"/>
-      <c r="C5" s="81"/>
-      <c r="D5" s="81"/>
-      <c r="E5" s="81"/>
+      <c r="B5" s="92"/>
+      <c r="C5" s="92"/>
+      <c r="D5" s="92"/>
+      <c r="E5" s="92"/>
       <c r="F5" s="5"/>
-      <c r="G5" s="82" t="s">
+      <c r="G5" s="93" t="s">
         <v>46</v>
       </c>
-      <c r="H5" s="83"/>
-      <c r="I5" s="83"/>
-      <c r="J5" s="83"/>
-      <c r="K5" s="84"/>
+      <c r="H5" s="94"/>
+      <c r="I5" s="94"/>
+      <c r="J5" s="94"/>
+      <c r="K5" s="95"/>
       <c r="L5" s="60"/>
       <c r="M5" s="5"/>
-      <c r="N5" s="82" t="s">
+      <c r="N5" s="93" t="s">
         <v>51</v>
       </c>
-      <c r="O5" s="83"/>
-      <c r="P5" s="83"/>
-      <c r="Q5" s="83"/>
-      <c r="R5" s="84"/>
+      <c r="O5" s="94"/>
+      <c r="P5" s="94"/>
+      <c r="Q5" s="94"/>
+      <c r="R5" s="95"/>
     </row>
     <row r="7" spans="1:18" ht="15.95" customHeight="1">
       <c r="A7" s="74" t="s">
@@ -19716,79 +19740,79 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I21" activeCellId="2" sqref="C21:C32 F21:F32 I21:I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:18" ht="20.25">
-      <c r="A1" s="97" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="98"/>
-      <c r="C1" s="98"/>
-      <c r="D1" s="98"/>
-      <c r="E1" s="98"/>
-      <c r="F1" s="98"/>
-      <c r="G1" s="98"/>
-      <c r="H1" s="98"/>
-      <c r="I1" s="98"/>
-      <c r="J1" s="98"/>
-      <c r="K1" s="99"/>
-      <c r="L1" s="98"/>
-      <c r="M1" s="98"/>
-      <c r="N1" s="98"/>
-      <c r="O1" s="98"/>
-      <c r="P1" s="98"/>
-      <c r="Q1" s="98"/>
-      <c r="R1" s="99"/>
+      <c r="A1" s="88" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="89"/>
+      <c r="C1" s="89"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="89"/>
+      <c r="F1" s="89"/>
+      <c r="G1" s="89"/>
+      <c r="H1" s="89"/>
+      <c r="I1" s="89"/>
+      <c r="J1" s="89"/>
+      <c r="K1" s="90"/>
+      <c r="L1" s="89"/>
+      <c r="M1" s="89"/>
+      <c r="N1" s="89"/>
+      <c r="O1" s="89"/>
+      <c r="P1" s="89"/>
+      <c r="Q1" s="89"/>
+      <c r="R1" s="90"/>
     </row>
     <row r="2" spans="1:18" ht="32.1" customHeight="1">
-      <c r="A2" s="89" t="s">
+      <c r="A2" s="80" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="90"/>
-      <c r="C2" s="90"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="91" t="s">
+      <c r="E2" s="82" t="s">
         <v>45</v>
       </c>
-      <c r="F2" s="91"/>
-      <c r="G2" s="91"/>
-      <c r="H2" s="91"/>
-      <c r="I2" s="91"/>
-      <c r="J2" s="91"/>
-      <c r="K2" s="92"/>
+      <c r="F2" s="82"/>
+      <c r="G2" s="82"/>
+      <c r="H2" s="82"/>
+      <c r="I2" s="82"/>
+      <c r="J2" s="82"/>
+      <c r="K2" s="83"/>
       <c r="L2" s="1"/>
-      <c r="M2" s="91"/>
-      <c r="N2" s="91"/>
-      <c r="O2" s="91"/>
-      <c r="P2" s="91"/>
-      <c r="Q2" s="91"/>
-      <c r="R2" s="92"/>
+      <c r="M2" s="82"/>
+      <c r="N2" s="82"/>
+      <c r="O2" s="82"/>
+      <c r="P2" s="82"/>
+      <c r="Q2" s="82"/>
+      <c r="R2" s="83"/>
     </row>
     <row r="3" spans="1:18">
-      <c r="A3" s="95" t="s">
+      <c r="A3" s="86" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="96"/>
-      <c r="C3" s="96"/>
+      <c r="B3" s="87"/>
+      <c r="C3" s="87"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="93"/>
-      <c r="J3" s="93"/>
-      <c r="K3" s="94"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="84"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="84"/>
+      <c r="J3" s="84"/>
+      <c r="K3" s="85"/>
       <c r="L3" s="2"/>
-      <c r="M3" s="93"/>
-      <c r="N3" s="93"/>
-      <c r="O3" s="93"/>
-      <c r="P3" s="93"/>
-      <c r="Q3" s="93"/>
-      <c r="R3" s="94"/>
+      <c r="M3" s="84"/>
+      <c r="N3" s="84"/>
+      <c r="O3" s="84"/>
+      <c r="P3" s="84"/>
+      <c r="Q3" s="84"/>
+      <c r="R3" s="85"/>
     </row>
     <row r="4" spans="1:18">
       <c r="A4" s="3"/>
@@ -19811,30 +19835,30 @@
       <c r="R4" s="4"/>
     </row>
     <row r="5" spans="1:18">
-      <c r="A5" s="80" t="s">
+      <c r="A5" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="81"/>
-      <c r="C5" s="81"/>
-      <c r="D5" s="81"/>
-      <c r="E5" s="81"/>
+      <c r="B5" s="92"/>
+      <c r="C5" s="92"/>
+      <c r="D5" s="92"/>
+      <c r="E5" s="92"/>
       <c r="F5" s="5"/>
-      <c r="G5" s="82" t="s">
+      <c r="G5" s="93" t="s">
         <v>42</v>
       </c>
-      <c r="H5" s="83"/>
-      <c r="I5" s="83"/>
-      <c r="J5" s="83"/>
-      <c r="K5" s="84"/>
+      <c r="H5" s="94"/>
+      <c r="I5" s="94"/>
+      <c r="J5" s="94"/>
+      <c r="K5" s="95"/>
       <c r="L5" s="60"/>
       <c r="M5" s="5"/>
-      <c r="N5" s="82" t="s">
+      <c r="N5" s="93" t="s">
         <v>50</v>
       </c>
-      <c r="O5" s="83"/>
-      <c r="P5" s="83"/>
-      <c r="Q5" s="83"/>
-      <c r="R5" s="84"/>
+      <c r="O5" s="94"/>
+      <c r="P5" s="94"/>
+      <c r="Q5" s="94"/>
+      <c r="R5" s="95"/>
     </row>
     <row r="7" spans="1:18" ht="15.95" customHeight="1">
       <c r="A7" s="74" t="s">
@@ -20926,49 +20950,49 @@
   <dimension ref="A1:R32"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="K21" sqref="K21:K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:18" ht="20.25">
-      <c r="A1" s="97" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="98"/>
-      <c r="C1" s="98"/>
-      <c r="D1" s="98"/>
-      <c r="E1" s="98"/>
-      <c r="F1" s="98"/>
-      <c r="G1" s="98"/>
-      <c r="H1" s="98"/>
-      <c r="I1" s="98"/>
-      <c r="J1" s="98"/>
-      <c r="K1" s="99"/>
-      <c r="L1" s="98"/>
-      <c r="M1" s="98"/>
-      <c r="N1" s="98"/>
-      <c r="O1" s="98"/>
-      <c r="P1" s="98"/>
-      <c r="Q1" s="98"/>
-      <c r="R1" s="99"/>
+      <c r="A1" s="88" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="89"/>
+      <c r="C1" s="89"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="89"/>
+      <c r="F1" s="89"/>
+      <c r="G1" s="89"/>
+      <c r="H1" s="89"/>
+      <c r="I1" s="89"/>
+      <c r="J1" s="89"/>
+      <c r="K1" s="90"/>
+      <c r="L1" s="89"/>
+      <c r="M1" s="89"/>
+      <c r="N1" s="89"/>
+      <c r="O1" s="89"/>
+      <c r="P1" s="89"/>
+      <c r="Q1" s="89"/>
+      <c r="R1" s="90"/>
     </row>
     <row r="2" spans="1:18" ht="32.1" customHeight="1">
-      <c r="A2" s="89" t="s">
+      <c r="A2" s="80" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="90"/>
-      <c r="C2" s="90"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="91" t="s">
+      <c r="E2" s="82" t="s">
         <v>60</v>
       </c>
-      <c r="F2" s="91"/>
-      <c r="G2" s="91"/>
-      <c r="H2" s="91"/>
-      <c r="I2" s="91"/>
-      <c r="J2" s="91"/>
-      <c r="K2" s="92"/>
+      <c r="F2" s="82"/>
+      <c r="G2" s="82"/>
+      <c r="H2" s="82"/>
+      <c r="I2" s="82"/>
+      <c r="J2" s="82"/>
+      <c r="K2" s="83"/>
       <c r="L2" s="1"/>
       <c r="M2" s="100"/>
       <c r="N2" s="100"/>
@@ -20978,19 +21002,19 @@
       <c r="R2" s="101"/>
     </row>
     <row r="3" spans="1:18">
-      <c r="A3" s="95" t="s">
+      <c r="A3" s="86" t="s">
         <v>55</v>
       </c>
-      <c r="B3" s="96"/>
-      <c r="C3" s="96"/>
+      <c r="B3" s="87"/>
+      <c r="C3" s="87"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="93"/>
-      <c r="J3" s="93"/>
-      <c r="K3" s="94"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="84"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="84"/>
+      <c r="J3" s="84"/>
+      <c r="K3" s="85"/>
       <c r="L3" s="2"/>
       <c r="M3" s="102"/>
       <c r="N3" s="102"/>
@@ -21020,30 +21044,30 @@
       <c r="R4" s="4"/>
     </row>
     <row r="5" spans="1:18">
-      <c r="A5" s="80" t="s">
+      <c r="A5" s="91" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="81"/>
-      <c r="C5" s="81"/>
-      <c r="D5" s="81"/>
-      <c r="E5" s="81"/>
+      <c r="B5" s="92"/>
+      <c r="C5" s="92"/>
+      <c r="D5" s="92"/>
+      <c r="E5" s="92"/>
       <c r="F5" s="5"/>
-      <c r="G5" s="82" t="s">
+      <c r="G5" s="93" t="s">
         <v>59</v>
       </c>
-      <c r="H5" s="83"/>
-      <c r="I5" s="83"/>
-      <c r="J5" s="83"/>
-      <c r="K5" s="84"/>
+      <c r="H5" s="94"/>
+      <c r="I5" s="94"/>
+      <c r="J5" s="94"/>
+      <c r="K5" s="95"/>
       <c r="L5" s="60"/>
       <c r="M5" s="5"/>
-      <c r="N5" s="82" t="s">
+      <c r="N5" s="93" t="s">
         <v>62</v>
       </c>
-      <c r="O5" s="83"/>
-      <c r="P5" s="83"/>
-      <c r="Q5" s="83"/>
-      <c r="R5" s="84"/>
+      <c r="O5" s="94"/>
+      <c r="P5" s="94"/>
+      <c r="Q5" s="94"/>
+      <c r="R5" s="95"/>
     </row>
     <row r="7" spans="1:18" ht="15.95" customHeight="1">
       <c r="A7" s="74" t="s">
@@ -22081,78 +22105,78 @@
   <dimension ref="A1:R32"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="K21" sqref="K21:K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:18" ht="20.25">
-      <c r="A1" s="97" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="98"/>
-      <c r="C1" s="98"/>
-      <c r="D1" s="98"/>
-      <c r="E1" s="98"/>
-      <c r="F1" s="98"/>
-      <c r="G1" s="98"/>
-      <c r="H1" s="98"/>
-      <c r="I1" s="98"/>
-      <c r="J1" s="98"/>
-      <c r="K1" s="99"/>
-      <c r="L1" s="98"/>
-      <c r="M1" s="98"/>
-      <c r="N1" s="98"/>
-      <c r="O1" s="98"/>
-      <c r="P1" s="98"/>
-      <c r="Q1" s="98"/>
-      <c r="R1" s="99"/>
+      <c r="A1" s="88" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="89"/>
+      <c r="C1" s="89"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="89"/>
+      <c r="F1" s="89"/>
+      <c r="G1" s="89"/>
+      <c r="H1" s="89"/>
+      <c r="I1" s="89"/>
+      <c r="J1" s="89"/>
+      <c r="K1" s="90"/>
+      <c r="L1" s="89"/>
+      <c r="M1" s="89"/>
+      <c r="N1" s="89"/>
+      <c r="O1" s="89"/>
+      <c r="P1" s="89"/>
+      <c r="Q1" s="89"/>
+      <c r="R1" s="90"/>
     </row>
     <row r="2" spans="1:18" ht="32.1" customHeight="1">
-      <c r="A2" s="89" t="s">
+      <c r="A2" s="80" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="90"/>
-      <c r="C2" s="90"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="91" t="s">
+      <c r="E2" s="82" t="s">
         <v>58</v>
       </c>
-      <c r="F2" s="91"/>
-      <c r="G2" s="91"/>
-      <c r="H2" s="91"/>
-      <c r="I2" s="91"/>
-      <c r="J2" s="91"/>
-      <c r="K2" s="92"/>
+      <c r="F2" s="82"/>
+      <c r="G2" s="82"/>
+      <c r="H2" s="82"/>
+      <c r="I2" s="82"/>
+      <c r="J2" s="82"/>
+      <c r="K2" s="83"/>
       <c r="L2" s="1"/>
-      <c r="M2" s="91"/>
-      <c r="N2" s="91"/>
-      <c r="O2" s="91"/>
-      <c r="P2" s="91"/>
-      <c r="Q2" s="91"/>
-      <c r="R2" s="92"/>
+      <c r="M2" s="82"/>
+      <c r="N2" s="82"/>
+      <c r="O2" s="82"/>
+      <c r="P2" s="82"/>
+      <c r="Q2" s="82"/>
+      <c r="R2" s="83"/>
     </row>
     <row r="3" spans="1:18">
-      <c r="A3" s="95" t="s">
+      <c r="A3" s="86" t="s">
         <v>55</v>
       </c>
-      <c r="B3" s="96"/>
-      <c r="C3" s="96"/>
+      <c r="B3" s="87"/>
+      <c r="C3" s="87"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="93"/>
-      <c r="J3" s="93"/>
-      <c r="K3" s="94"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="84"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="84"/>
+      <c r="J3" s="84"/>
+      <c r="K3" s="85"/>
       <c r="L3" s="2"/>
-      <c r="M3" s="93"/>
-      <c r="N3" s="93"/>
-      <c r="O3" s="93"/>
-      <c r="P3" s="93"/>
-      <c r="Q3" s="93"/>
-      <c r="R3" s="94"/>
+      <c r="M3" s="84"/>
+      <c r="N3" s="84"/>
+      <c r="O3" s="84"/>
+      <c r="P3" s="84"/>
+      <c r="Q3" s="84"/>
+      <c r="R3" s="85"/>
     </row>
     <row r="4" spans="1:18">
       <c r="A4" s="3"/>
@@ -22175,30 +22199,30 @@
       <c r="R4" s="4"/>
     </row>
     <row r="5" spans="1:18">
-      <c r="A5" s="80" t="s">
+      <c r="A5" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="81"/>
-      <c r="C5" s="81"/>
-      <c r="D5" s="81"/>
-      <c r="E5" s="81"/>
+      <c r="B5" s="92"/>
+      <c r="C5" s="92"/>
+      <c r="D5" s="92"/>
+      <c r="E5" s="92"/>
       <c r="F5" s="5"/>
-      <c r="G5" s="82" t="s">
+      <c r="G5" s="93" t="s">
         <v>57</v>
       </c>
-      <c r="H5" s="83"/>
-      <c r="I5" s="83"/>
-      <c r="J5" s="83"/>
-      <c r="K5" s="84"/>
+      <c r="H5" s="94"/>
+      <c r="I5" s="94"/>
+      <c r="J5" s="94"/>
+      <c r="K5" s="95"/>
       <c r="L5" s="60"/>
       <c r="M5" s="5"/>
-      <c r="N5" s="82" t="s">
+      <c r="N5" s="93" t="s">
         <v>61</v>
       </c>
-      <c r="O5" s="83"/>
-      <c r="P5" s="83"/>
-      <c r="Q5" s="83"/>
-      <c r="R5" s="84"/>
+      <c r="O5" s="94"/>
+      <c r="P5" s="94"/>
+      <c r="Q5" s="94"/>
+      <c r="R5" s="95"/>
     </row>
     <row r="8" spans="1:18" ht="31.5">
       <c r="A8" s="74" t="s">
@@ -23246,50 +23270,50 @@
       <c r="R1" s="106"/>
     </row>
     <row r="2" spans="1:18" ht="32.1" customHeight="1">
-      <c r="A2" s="89" t="s">
+      <c r="A2" s="80" t="s">
         <v>131</v>
       </c>
-      <c r="B2" s="90"/>
-      <c r="C2" s="90"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="91" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="91"/>
-      <c r="G2" s="91"/>
-      <c r="H2" s="91"/>
-      <c r="I2" s="91"/>
-      <c r="J2" s="91"/>
-      <c r="K2" s="92"/>
+      <c r="E2" s="82" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="82"/>
+      <c r="G2" s="82"/>
+      <c r="H2" s="82"/>
+      <c r="I2" s="82"/>
+      <c r="J2" s="82"/>
+      <c r="K2" s="83"/>
       <c r="L2" s="1"/>
-      <c r="M2" s="91"/>
-      <c r="N2" s="91"/>
-      <c r="O2" s="91"/>
-      <c r="P2" s="91"/>
-      <c r="Q2" s="91"/>
-      <c r="R2" s="92"/>
+      <c r="M2" s="82"/>
+      <c r="N2" s="82"/>
+      <c r="O2" s="82"/>
+      <c r="P2" s="82"/>
+      <c r="Q2" s="82"/>
+      <c r="R2" s="83"/>
     </row>
     <row r="3" spans="1:18">
-      <c r="A3" s="95" t="s">
+      <c r="A3" s="86" t="s">
         <v>132</v>
       </c>
-      <c r="B3" s="96"/>
-      <c r="C3" s="96"/>
+      <c r="B3" s="87"/>
+      <c r="C3" s="87"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="93"/>
-      <c r="J3" s="93"/>
-      <c r="K3" s="94"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="84"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="84"/>
+      <c r="J3" s="84"/>
+      <c r="K3" s="85"/>
       <c r="L3" s="2"/>
-      <c r="M3" s="93"/>
-      <c r="N3" s="93"/>
-      <c r="O3" s="93"/>
-      <c r="P3" s="93"/>
-      <c r="Q3" s="93"/>
-      <c r="R3" s="94"/>
+      <c r="M3" s="84"/>
+      <c r="N3" s="84"/>
+      <c r="O3" s="84"/>
+      <c r="P3" s="84"/>
+      <c r="Q3" s="84"/>
+      <c r="R3" s="85"/>
     </row>
     <row r="4" spans="1:18">
       <c r="A4" s="3"/>
@@ -23312,30 +23336,30 @@
       <c r="R4" s="4"/>
     </row>
     <row r="5" spans="1:18">
-      <c r="A5" s="80" t="s">
+      <c r="A5" s="91" t="s">
         <v>133</v>
       </c>
-      <c r="B5" s="81"/>
-      <c r="C5" s="81"/>
-      <c r="D5" s="81"/>
-      <c r="E5" s="81"/>
+      <c r="B5" s="92"/>
+      <c r="C5" s="92"/>
+      <c r="D5" s="92"/>
+      <c r="E5" s="92"/>
       <c r="F5" s="5"/>
-      <c r="G5" s="81" t="s">
+      <c r="G5" s="92" t="s">
         <v>134</v>
       </c>
-      <c r="H5" s="83"/>
-      <c r="I5" s="83"/>
-      <c r="J5" s="83"/>
-      <c r="K5" s="84"/>
+      <c r="H5" s="94"/>
+      <c r="I5" s="94"/>
+      <c r="J5" s="94"/>
+      <c r="K5" s="95"/>
       <c r="L5" s="60"/>
       <c r="M5" s="5"/>
-      <c r="N5" s="81" t="s">
+      <c r="N5" s="92" t="s">
         <v>135</v>
       </c>
-      <c r="O5" s="83"/>
-      <c r="P5" s="83"/>
-      <c r="Q5" s="83"/>
-      <c r="R5" s="84"/>
+      <c r="O5" s="94"/>
+      <c r="P5" s="94"/>
+      <c r="Q5" s="94"/>
+      <c r="R5" s="95"/>
     </row>
     <row r="7" spans="1:18" ht="15.95" customHeight="1">
       <c r="A7" s="74" t="s">
@@ -24631,19 +24655,19 @@
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:23" ht="20.25">
-      <c r="A1" s="97" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="98"/>
-      <c r="C1" s="98"/>
-      <c r="D1" s="98"/>
-      <c r="E1" s="98"/>
-      <c r="F1" s="98"/>
-      <c r="G1" s="98"/>
-      <c r="H1" s="98"/>
-      <c r="I1" s="98"/>
-      <c r="J1" s="98"/>
-      <c r="K1" s="99"/>
+      <c r="A1" s="88" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="89"/>
+      <c r="C1" s="89"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="89"/>
+      <c r="F1" s="89"/>
+      <c r="G1" s="89"/>
+      <c r="H1" s="89"/>
+      <c r="I1" s="89"/>
+      <c r="J1" s="89"/>
+      <c r="K1" s="90"/>
       <c r="L1" s="38"/>
       <c r="M1" s="53"/>
       <c r="N1" s="53"/>
@@ -24658,21 +24682,21 @@
       <c r="W1" s="53"/>
     </row>
     <row r="2" spans="1:23" ht="33" customHeight="1">
-      <c r="A2" s="89" t="s">
+      <c r="A2" s="80" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="90"/>
-      <c r="C2" s="90"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="91" t="s">
+      <c r="E2" s="82" t="s">
         <v>107</v>
       </c>
-      <c r="F2" s="91"/>
-      <c r="G2" s="91"/>
-      <c r="H2" s="91"/>
-      <c r="I2" s="91"/>
-      <c r="J2" s="91"/>
-      <c r="K2" s="92"/>
+      <c r="F2" s="82"/>
+      <c r="G2" s="82"/>
+      <c r="H2" s="82"/>
+      <c r="I2" s="82"/>
+      <c r="J2" s="82"/>
+      <c r="K2" s="83"/>
       <c r="L2" s="38"/>
       <c r="M2" s="54"/>
       <c r="N2" s="54"/>
@@ -24687,19 +24711,19 @@
       <c r="W2" s="56"/>
     </row>
     <row r="3" spans="1:23" ht="15.95" customHeight="1">
-      <c r="A3" s="95" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="96"/>
-      <c r="C3" s="96"/>
+      <c r="A3" s="86" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="87"/>
+      <c r="C3" s="87"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="93"/>
-      <c r="J3" s="93"/>
-      <c r="K3" s="94"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="84"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="84"/>
+      <c r="J3" s="84"/>
+      <c r="K3" s="85"/>
       <c r="L3" s="38"/>
       <c r="M3" s="57"/>
       <c r="N3" s="57"/>
@@ -24739,21 +24763,21 @@
       <c r="W4" s="56"/>
     </row>
     <row r="5" spans="1:23" ht="15.95" customHeight="1">
-      <c r="A5" s="80" t="s">
+      <c r="A5" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="81"/>
-      <c r="C5" s="81"/>
-      <c r="D5" s="81"/>
-      <c r="E5" s="81"/>
+      <c r="B5" s="92"/>
+      <c r="C5" s="92"/>
+      <c r="D5" s="92"/>
+      <c r="E5" s="92"/>
       <c r="F5" s="5"/>
-      <c r="G5" s="82" t="s">
+      <c r="G5" s="93" t="s">
         <v>106</v>
       </c>
-      <c r="H5" s="83"/>
-      <c r="I5" s="83"/>
-      <c r="J5" s="83"/>
-      <c r="K5" s="84"/>
+      <c r="H5" s="94"/>
+      <c r="I5" s="94"/>
+      <c r="J5" s="94"/>
+      <c r="K5" s="95"/>
       <c r="L5" s="38"/>
       <c r="M5" s="58"/>
       <c r="N5" s="58"/>
@@ -24782,21 +24806,21 @@
       <c r="W6" s="55"/>
     </row>
     <row r="7" spans="1:23" ht="15.95" customHeight="1">
-      <c r="B7" s="85" t="s">
+      <c r="B7" s="96" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="85"/>
-      <c r="D7" s="85"/>
-      <c r="E7" s="86" t="s">
+      <c r="C7" s="96"/>
+      <c r="D7" s="96"/>
+      <c r="E7" s="97" t="s">
         <v>105</v>
       </c>
-      <c r="F7" s="85"/>
-      <c r="G7" s="87"/>
-      <c r="H7" s="85" t="s">
+      <c r="F7" s="96"/>
+      <c r="G7" s="98"/>
+      <c r="H7" s="96" t="s">
         <v>4</v>
       </c>
-      <c r="I7" s="85"/>
-      <c r="J7" s="88"/>
+      <c r="I7" s="96"/>
+      <c r="J7" s="99"/>
       <c r="K7" s="6"/>
       <c r="L7" s="38"/>
       <c r="M7" s="54"/>
@@ -25317,27 +25341,27 @@
       <c r="G1" s="48"/>
       <c r="H1" s="49"/>
       <c r="I1" s="38"/>
-      <c r="O1" s="98"/>
-      <c r="P1" s="98"/>
-      <c r="Q1" s="98"/>
-      <c r="R1" s="98"/>
-      <c r="S1" s="98"/>
-      <c r="T1" s="98"/>
-      <c r="U1" s="99"/>
+      <c r="O1" s="89"/>
+      <c r="P1" s="89"/>
+      <c r="Q1" s="89"/>
+      <c r="R1" s="89"/>
+      <c r="S1" s="89"/>
+      <c r="T1" s="89"/>
+      <c r="U1" s="90"/>
     </row>
     <row r="2" spans="1:21" ht="32.1" customHeight="1">
       <c r="A2" s="79" t="s">
         <v>111</v>
       </c>
-      <c r="B2" s="91" t="s">
+      <c r="B2" s="82" t="s">
         <v>115</v>
       </c>
-      <c r="C2" s="91"/>
-      <c r="D2" s="91"/>
-      <c r="E2" s="91"/>
-      <c r="F2" s="91"/>
-      <c r="G2" s="91"/>
-      <c r="H2" s="92"/>
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="82"/>
+      <c r="G2" s="82"/>
+      <c r="H2" s="83"/>
       <c r="I2" s="38"/>
       <c r="O2" s="1"/>
       <c r="P2" s="100"/>
@@ -25351,13 +25375,13 @@
       <c r="A3" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="B3" s="93"/>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="94"/>
+      <c r="B3" s="84"/>
+      <c r="C3" s="84"/>
+      <c r="D3" s="84"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="84"/>
+      <c r="H3" s="85"/>
       <c r="I3" s="38"/>
       <c r="O3" s="2"/>
       <c r="P3" s="102"/>
@@ -25401,13 +25425,13 @@
       <c r="I5" s="38"/>
       <c r="O5" s="60"/>
       <c r="P5" s="5"/>
-      <c r="Q5" s="82" t="s">
+      <c r="Q5" s="93" t="s">
         <v>51</v>
       </c>
-      <c r="R5" s="83"/>
-      <c r="S5" s="83"/>
-      <c r="T5" s="83"/>
-      <c r="U5" s="84"/>
+      <c r="R5" s="94"/>
+      <c r="S5" s="94"/>
+      <c r="T5" s="94"/>
+      <c r="U5" s="95"/>
     </row>
     <row r="6" spans="1:21">
       <c r="I6" s="38"/>
@@ -25538,7 +25562,7 @@
       <c r="L9" s="1"/>
       <c r="M9" s="13"/>
       <c r="N9" s="1">
-        <f>SUM(B9:M9)</f>
+        <f t="shared" ref="N9:N32" si="0">SUM(B9:M9)</f>
         <v>18</v>
       </c>
       <c r="O9" s="6">
@@ -25558,7 +25582,7 @@
       </c>
       <c r="T9" s="18"/>
       <c r="U9" s="14">
-        <f t="shared" ref="U9:U32" si="0">SUM(O9:T9)</f>
+        <f t="shared" ref="U9:U32" si="1">SUM(O9:T9)</f>
         <v>282</v>
       </c>
     </row>
@@ -25589,7 +25613,7 @@
       </c>
       <c r="M10" s="25"/>
       <c r="N10" s="1">
-        <f>SUM(B10:M10)</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="O10" s="26">
@@ -25607,7 +25631,7 @@
       <c r="S10" s="22"/>
       <c r="T10" s="22"/>
       <c r="U10" s="26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>327</v>
       </c>
     </row>
@@ -25638,7 +25662,7 @@
       </c>
       <c r="M11" s="13"/>
       <c r="N11" s="1">
-        <f>SUM(B11:M11)</f>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="O11" s="14">
@@ -25656,7 +25680,7 @@
       <c r="S11" s="15"/>
       <c r="T11" s="15"/>
       <c r="U11" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>437</v>
       </c>
     </row>
@@ -25687,7 +25711,7 @@
       </c>
       <c r="M12" s="25"/>
       <c r="N12" s="1">
-        <f>SUM(B12:M12)</f>
+        <f t="shared" si="0"/>
         <v>33</v>
       </c>
       <c r="O12" s="26">
@@ -25705,7 +25729,7 @@
       <c r="S12" s="22"/>
       <c r="T12" s="22"/>
       <c r="U12" s="26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>436</v>
       </c>
     </row>
@@ -25736,7 +25760,7 @@
       </c>
       <c r="M13" s="13"/>
       <c r="N13" s="1">
-        <f>SUM(B13:M13)</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="O13" s="14">
@@ -25754,7 +25778,7 @@
       <c r="S13" s="15"/>
       <c r="T13" s="15"/>
       <c r="U13" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>596</v>
       </c>
     </row>
@@ -25785,7 +25809,7 @@
       </c>
       <c r="M14" s="25"/>
       <c r="N14" s="1">
-        <f>SUM(B14:M14)</f>
+        <f t="shared" si="0"/>
         <v>44</v>
       </c>
       <c r="O14" s="26">
@@ -25803,7 +25827,7 @@
       <c r="S14" s="22"/>
       <c r="T14" s="22"/>
       <c r="U14" s="26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>476</v>
       </c>
     </row>
@@ -25830,7 +25854,7 @@
       <c r="L15" s="1"/>
       <c r="M15" s="13"/>
       <c r="N15" s="1">
-        <f>SUM(B15:M15)</f>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="O15" s="14">
@@ -25848,7 +25872,7 @@
       <c r="S15" s="15"/>
       <c r="T15" s="15"/>
       <c r="U15" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>519</v>
       </c>
     </row>
@@ -25873,7 +25897,7 @@
       <c r="L16" s="23"/>
       <c r="M16" s="25"/>
       <c r="N16" s="1">
-        <f>SUM(B16:M16)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="O16" s="26">
@@ -25891,7 +25915,7 @@
       <c r="S16" s="22"/>
       <c r="T16" s="22"/>
       <c r="U16" s="26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>500</v>
       </c>
     </row>
@@ -25918,7 +25942,7 @@
       </c>
       <c r="M17" s="13"/>
       <c r="N17" s="1">
-        <f>SUM(B17:M17)</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="O17" s="14">
@@ -25936,7 +25960,7 @@
       <c r="S17" s="15"/>
       <c r="T17" s="15"/>
       <c r="U17" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>497</v>
       </c>
     </row>
@@ -25969,7 +25993,7 @@
       </c>
       <c r="M18" s="25"/>
       <c r="N18" s="1">
-        <f>SUM(B18:M18)</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="O18" s="26">
@@ -25987,7 +26011,7 @@
       <c r="S18" s="22"/>
       <c r="T18" s="22"/>
       <c r="U18" s="26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>467</v>
       </c>
     </row>
@@ -26016,7 +26040,7 @@
       </c>
       <c r="M19" s="13"/>
       <c r="N19" s="1">
-        <f>SUM(B19:M19)</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="O19" s="14">
@@ -26034,7 +26058,7 @@
       <c r="S19" s="15"/>
       <c r="T19" s="15"/>
       <c r="U19" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>407</v>
       </c>
     </row>
@@ -26063,7 +26087,7 @@
       </c>
       <c r="M20" s="32"/>
       <c r="N20" s="1">
-        <f>SUM(B20:M20)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="O20" s="33">
@@ -26081,7 +26105,7 @@
       <c r="S20" s="29"/>
       <c r="T20" s="29"/>
       <c r="U20" s="33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>382</v>
       </c>
     </row>
@@ -26106,7 +26130,7 @@
       <c r="L21" s="1"/>
       <c r="M21" s="13"/>
       <c r="N21" s="1">
-        <f>SUM(B21:M21)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="O21" s="6">
@@ -26124,7 +26148,7 @@
       <c r="S21" s="18"/>
       <c r="T21" s="18"/>
       <c r="U21" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>289</v>
       </c>
     </row>
@@ -26151,7 +26175,7 @@
       </c>
       <c r="M22" s="25"/>
       <c r="N22" s="1">
-        <f>SUM(B22:M22)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="O22" s="26">
@@ -26169,7 +26193,7 @@
       <c r="S22" s="22"/>
       <c r="T22" s="22"/>
       <c r="U22" s="26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>285</v>
       </c>
     </row>
@@ -26194,7 +26218,7 @@
       <c r="L23" s="1"/>
       <c r="M23" s="13"/>
       <c r="N23" s="1">
-        <f>SUM(B23:M23)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="O23" s="14">
@@ -26212,7 +26236,7 @@
       </c>
       <c r="T23" s="15"/>
       <c r="U23" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>295</v>
       </c>
     </row>
@@ -26237,7 +26261,7 @@
       <c r="L24" s="23"/>
       <c r="M24" s="25"/>
       <c r="N24" s="1">
-        <f>SUM(B24:M24)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="O24" s="26">
@@ -26251,7 +26275,7 @@
       <c r="S24" s="22"/>
       <c r="T24" s="22"/>
       <c r="U24" s="26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>329</v>
       </c>
     </row>
@@ -26280,7 +26304,7 @@
       </c>
       <c r="M25" s="13"/>
       <c r="N25" s="1">
-        <f>SUM(B25:M25)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="O25" s="14">
@@ -26298,7 +26322,7 @@
       <c r="S25" s="15"/>
       <c r="T25" s="15"/>
       <c r="U25" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>338</v>
       </c>
     </row>
@@ -26329,7 +26353,7 @@
       </c>
       <c r="M26" s="25"/>
       <c r="N26" s="1">
-        <f>SUM(B26:M26)</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="O26" s="26">
@@ -26347,7 +26371,7 @@
       <c r="S26" s="22"/>
       <c r="T26" s="22"/>
       <c r="U26" s="26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>333</v>
       </c>
     </row>
@@ -26378,7 +26402,7 @@
       </c>
       <c r="M27" s="13"/>
       <c r="N27" s="1">
-        <f>SUM(B27:M27)</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="O27" s="14">
@@ -26398,7 +26422,7 @@
       </c>
       <c r="T27" s="15"/>
       <c r="U27" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>337</v>
       </c>
     </row>
@@ -26427,7 +26451,7 @@
       <c r="L28" s="23"/>
       <c r="M28" s="25"/>
       <c r="N28" s="1">
-        <f>SUM(B28:M28)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="O28" s="26">
@@ -26445,7 +26469,7 @@
       </c>
       <c r="T28" s="22"/>
       <c r="U28" s="26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>313</v>
       </c>
     </row>
@@ -26472,7 +26496,7 @@
       <c r="L29" s="1"/>
       <c r="M29" s="13"/>
       <c r="N29" s="1">
-        <f>SUM(B29:M29)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="O29" s="14">
@@ -26488,7 +26512,7 @@
       <c r="S29" s="15"/>
       <c r="T29" s="15"/>
       <c r="U29" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>296</v>
       </c>
     </row>
@@ -26519,7 +26543,7 @@
       </c>
       <c r="M30" s="25"/>
       <c r="N30" s="1">
-        <f>SUM(B30:M30)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="O30" s="26">
@@ -26535,7 +26559,7 @@
       <c r="S30" s="22"/>
       <c r="T30" s="22"/>
       <c r="U30" s="26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>280</v>
       </c>
     </row>
@@ -26560,7 +26584,7 @@
       <c r="L31" s="1"/>
       <c r="M31" s="13"/>
       <c r="N31" s="1">
-        <f>SUM(B31:M31)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="O31" s="14">
@@ -26576,7 +26600,7 @@
       <c r="S31" s="15"/>
       <c r="T31" s="15"/>
       <c r="U31" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>287</v>
       </c>
     </row>
@@ -26601,7 +26625,7 @@
       <c r="L32" s="30"/>
       <c r="M32" s="32"/>
       <c r="N32" s="1">
-        <f>SUM(B32:M32)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="O32" s="33">
@@ -26617,7 +26641,7 @@
       <c r="S32" s="29"/>
       <c r="T32" s="29"/>
       <c r="U32" s="33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>239</v>
       </c>
     </row>

</xml_diff>